<commit_message>
S3 day 3 08/06/2021
</commit_message>
<xml_diff>
--- a/Daily Routine.xlsx
+++ b/Daily Routine.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91892\Desktop\Job Research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91892\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2C63ED-5A9D-4526-8D35-1D79C321F5BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E99E94C-D5A8-4E61-BB14-802B48CA5D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{50582D76-538B-40BA-B8A8-6D7BFB74E9F7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
   <si>
     <t>Date</t>
   </si>
@@ -154,6 +154,21 @@
   </si>
   <si>
     <t>Age/time and worl</t>
+  </si>
+  <si>
+    <t>05/08/2021 thru</t>
+  </si>
+  <si>
+    <t>solved 1 question</t>
+  </si>
+  <si>
+    <t>time and work</t>
+  </si>
+  <si>
+    <t>6/8/2021 Friday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solving 1 problem </t>
   </si>
 </sst>
 </file>
@@ -522,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63367EDB-8D7A-417D-BD80-0C36D5BBFFD0}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -747,6 +762,34 @@
         <v>42</v>
       </c>
     </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
S3 day 5 08/09/2021
</commit_message>
<xml_diff>
--- a/Daily Routine.xlsx
+++ b/Daily Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91892\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E99E94C-D5A8-4E61-BB14-802B48CA5D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787997EB-AF3A-47BC-B5B1-40549A7ED126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{50582D76-538B-40BA-B8A8-6D7BFB74E9F7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="60">
   <si>
     <t>Date</t>
   </si>
@@ -169,6 +169,42 @@
   </si>
   <si>
     <t xml:space="preserve">solving 1 problem </t>
+  </si>
+  <si>
+    <t>07/08/2021 Sat</t>
+  </si>
+  <si>
+    <t>solving many problems</t>
+  </si>
+  <si>
+    <t>8/8/2021 Sunday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Backtracking problem </t>
+  </si>
+  <si>
+    <t>nA</t>
+  </si>
+  <si>
+    <t>Na</t>
+  </si>
+  <si>
+    <t>Solvong appti problem</t>
+  </si>
+  <si>
+    <t>09/08/2021 Monday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 problem on back tracking </t>
+  </si>
+  <si>
+    <t>give contest of DIV 2</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>Solving ratio problem</t>
   </si>
 </sst>
 </file>
@@ -537,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63367EDB-8D7A-417D-BD80-0C36D5BBFFD0}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -790,6 +826,66 @@
         <v>47</v>
       </c>
     </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>